<commit_message>
show images with glide (firestore)
</commit_message>
<xml_diff>
--- a/Mobil alkalmazásfejlesztés projektmunka pontozás.xlsx
+++ b/Mobil alkalmazásfejlesztés projektmunka pontozás.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srkzgrg/Desktop/mobilalk-kotprog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA4E36B-5108-2B4C-991B-1FDFC0DB23E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DD212-67A2-A946-B058-C5B2197FB429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -156,14 +156,14 @@
     </r>
   </si>
   <si>
-    <t>c</t>
+    <t>Legalább egy olyan androidos erőforrás használata, amihez kell android permission</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -203,8 +203,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +227,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -295,6 +308,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -515,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -563,7 +580,7 @@
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="14">
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -574,7 +591,7 @@
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -585,7 +602,7 @@
       <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -596,7 +613,7 @@
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -607,7 +624,7 @@
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="14">
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -618,7 +635,7 @@
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="15">
         <v>3</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -629,7 +646,7 @@
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="14">
         <v>2</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -640,14 +657,14 @@
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="14">
         <v>2</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -659,7 +676,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="9">
@@ -669,8 +686,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="9">
@@ -684,7 +701,7 @@
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="14">
         <v>5</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -695,7 +712,7 @@
       <c r="A16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="14">
         <v>4</v>
       </c>
       <c r="C16" s="10" t="s">

</xml_diff>